<commit_message>
changed how date fields are detected updated models
</commit_message>
<xml_diff>
--- a/static/bulk_template.xlsx
+++ b/static/bulk_template.xlsx
@@ -8,12 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="SOP" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="PlasmidBatch" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Plasmid" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Plasmid" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="PlasmidBatch" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Primers" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Strain" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="CellLine" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Fermentation" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="StrainBatch" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="CellLine" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="CellLineBatch" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="CultureMedia" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="CultureMediaBatch" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Fermentation" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -454,7 +458,155 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>responsible</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Barcode</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>TubesLeft</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Mycoplasma</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Parent</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>responsible</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>RunDate</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Strain</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>responsible</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>CommonName</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Usage</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Antibiotic</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Batches</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -492,62 +644,6 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>Parent</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>responsible</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>CommonName</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Usage</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Antibiotic</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Location</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Batches</t>
         </is>
       </c>
     </row>
@@ -608,7 +704,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,17 +775,7 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>TubesLeft</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>TubeVolume</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Location</t>
+          <t>Batches</t>
         </is>
       </c>
     </row>
@@ -725,27 +811,27 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>CommonName</t>
+          <t>TubesLeft</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Usage</t>
+          <t>Barcode</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Species</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Genotype</t>
+          <t>SequenceVerified</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Parent</t>
         </is>
       </c>
     </row>
@@ -760,7 +846,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -781,12 +867,134 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>RunDate</t>
+          <t>CommonName</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Strain</t>
+          <t>Usage</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Species</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Batches</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>responsible</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Barcode</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>TubesLeft</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Mycoplasma</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Parent</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>responsible</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ProductName</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Vendor</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>CatalogNo</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Batches</t>
         </is>
       </c>
     </row>

</xml_diff>